<commit_message>
added parallel tests, webdriverManager in base class, multiple data provider management tests
</commit_message>
<xml_diff>
--- a/src/main/java/com/testdata/WtriteWebTableIntoXcel.xlsx
+++ b/src/main/java/com/testdata/WtriteWebTableIntoXcel.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="32">
   <si>
     <t>Company</t>
   </si>
@@ -51,8 +51,8 @@
     <t>FineshedAt</t>
   </si>
   <si>
-    <t>1571334563820
-Thu Oct 17 10:49:23 PDT 2019</t>
+    <t>1571855800605
+Wed Oct 23 11:36:40 PDT 2019</t>
   </si>
   <si>
     <t>Contact</t>
@@ -76,8 +76,8 @@
     <t>Giovanni Rovelli</t>
   </si>
   <si>
-    <t>1571334565652
-Thu Oct 17 10:49:25 PDT 2019</t>
+    <t>1571855802576
+Wed Oct 23 11:36:42 PDT 2019</t>
   </si>
   <si>
     <t>Country</t>
@@ -101,16 +101,36 @@
     <t>Italy</t>
   </si>
   <si>
-    <t>1571334566494
-Thu Oct 17 10:49:26 PDT 2019</t>
-  </si>
-  <si>
-    <t>1571334569471
-Thu Oct 17 10:49:29 PDT 2019</t>
-  </si>
-  <si>
-    <t>1571334570770
-Thu Oct 17 10:49:30 PDT 2019</t>
+    <t>1571855803803
+Wed Oct 23 11:36:43 PDT 2019</t>
+  </si>
+  <si>
+    <t>1571855810696
+Wed Oct 23 11:36:50 PDT 2019</t>
+  </si>
+  <si>
+    <t>1571855812034
+Wed Oct 23 11:36:52 PDT 2019</t>
+  </si>
+  <si>
+    <t>1571855967414
+Wed Oct 23 11:39:27 PDT 2019</t>
+  </si>
+  <si>
+    <t>1571855969248
+Wed Oct 23 11:39:29 PDT 2019</t>
+  </si>
+  <si>
+    <t>1571855971281
+Wed Oct 23 11:39:31 PDT 2019</t>
+  </si>
+  <si>
+    <t>1571855997720
+Wed Oct 23 11:39:57 PDT 2019</t>
+  </si>
+  <si>
+    <t>1571856027433
+Wed Oct 23 11:40:27 PDT 2019</t>
   </si>
 </sst>
 </file>
@@ -195,11 +215,25 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
@@ -237,7 +271,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -251,7 +285,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -259,6 +293,8 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="28.36328125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="11.1328125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="28.36328125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.1328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -268,16 +304,28 @@
       <c r="B1" t="s" s="2">
         <v>7</v>
       </c>
+      <c r="C1" t="s" s="15">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s" s="16">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -286,19 +334,34 @@
       <c r="B4" t="s">
         <v>8</v>
       </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -309,7 +372,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -317,6 +380,8 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="16.1328125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="11.1328125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.1328125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.1328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -326,16 +391,28 @@
       <c r="B1" t="s" s="4">
         <v>7</v>
       </c>
+      <c r="C1" t="s" s="17">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s" s="18">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -344,19 +421,34 @@
       <c r="B4" t="s">
         <v>16</v>
       </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>13</v>
       </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>14</v>
       </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -367,7 +459,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -375,6 +467,8 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="9.23828125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="11.1328125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.23828125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.1328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -384,16 +478,28 @@
       <c r="B1" t="s" s="6">
         <v>7</v>
       </c>
+      <c r="C1" t="s" s="19">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s" s="20">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -402,19 +508,34 @@
       <c r="B4" t="s">
         <v>24</v>
       </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
         <v>21</v>
       </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
         <v>22</v>
       </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
         <v>23</v>
       </c>
     </row>
@@ -425,7 +546,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -435,6 +556,10 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="16.1328125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="9.23828125" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="11.1328125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="28.36328125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.1328125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.23828125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.1328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -450,6 +575,18 @@
       <c r="D1" t="s" s="10">
         <v>7</v>
       </c>
+      <c r="E1" t="s" s="21">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s" s="22">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s" s="23">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s" s="24">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -461,6 +598,15 @@
       <c r="C2" t="s">
         <v>18</v>
       </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -472,6 +618,15 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -486,6 +641,18 @@
       <c r="D4" t="s">
         <v>25</v>
       </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -497,6 +664,15 @@
       <c r="C5" t="s">
         <v>21</v>
       </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -508,6 +684,15 @@
       <c r="C6" t="s">
         <v>22</v>
       </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -517,6 +702,15 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
         <v>23</v>
       </c>
     </row>
@@ -527,7 +721,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -536,7 +730,11 @@
     <col min="1" max="1" bestFit="true" customWidth="true" width="28.36328125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="16.1328125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="9.23828125" collapsed="true"/>
-    <col min="4" max="4" width="11.1328125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.1328125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="28.36328125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.1328125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.23828125" collapsed="true"/>
+    <col min="8" max="8" width="11.1328125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -552,6 +750,18 @@
       <c r="D1" t="s" s="14">
         <v>7</v>
       </c>
+      <c r="E1" t="s" s="25">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s" s="26">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s" s="27">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s" s="28">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -563,6 +773,15 @@
       <c r="C2" t="s">
         <v>18</v>
       </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -574,6 +793,15 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -588,6 +816,18 @@
       <c r="D4" t="s">
         <v>26</v>
       </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
@@ -599,6 +839,15 @@
       <c r="C5" t="s">
         <v>21</v>
       </c>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
@@ -610,6 +859,15 @@
       <c r="C6" t="s">
         <v>22</v>
       </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
@@ -619,6 +877,15 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>